<commit_message>
updated excel for simulator grapth
</commit_message>
<xml_diff>
--- a/dcycl/analysis/Simulator/simulator_distace.xlsx
+++ b/dcycl/analysis/Simulator/simulator_distace.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sapie\Creative Cloud Files\TUe\M1.2\cyclist-distance-crowdsourced\dcycl\analysis\Simulator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DA5ECDA-ECE6-44D0-AF30-56C532BD9D93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0B7BB2A-8B0A-4C4B-BDD1-CF577AEC3DC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4448" yWindow="4410" windowWidth="14385" windowHeight="7650" xr2:uid="{254CCC8E-036F-4719-AEB3-81A051663563}"/>
+    <workbookView xWindow="3360" yWindow="3967" windowWidth="14385" windowHeight="7650" xr2:uid="{254CCC8E-036F-4719-AEB3-81A051663563}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -442,7 +442,7 @@
   <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -616,7 +616,9 @@
       <c r="D7" s="1">
         <v>1.7243820000000001</v>
       </c>
-      <c r="E7" s="1"/>
+      <c r="E7" s="1">
+        <v>0</v>
+      </c>
       <c r="F7" s="1">
         <v>1.5914029999999999</v>
       </c>

</xml_diff>